<commit_message>
Imprort function done =)
</commit_message>
<xml_diff>
--- a/templates/address.xlsx
+++ b/templates/address.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>CONTACT_ID</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>DATE_OBSOLETE (dd-MMM-yyyy)</t>
+  </si>
+  <si>
+    <t>singparieowbf</t>
+  </si>
+  <si>
+    <t>wefiorefn</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,7 +500,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>123123</v>
@@ -514,7 +520,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>123123</v>

</xml_diff>